<commit_message>
Clean project for deployment
</commit_message>
<xml_diff>
--- a/Attendance_Report.xlsx
+++ b/Attendance_Report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,34 +483,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>02:48</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2026-02-28</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>8754</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ADESH DEHADE</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>02:51</t>
+          <t>04:39</t>
         </is>
       </c>
     </row>

</xml_diff>